<commit_message>
Update Tomos Targa LX
</commit_message>
<xml_diff>
--- a/Life/Tomos Targa LX.xlsx
+++ b/Life/Tomos Targa LX.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\twc1001\Life\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5081827-0BF1-4B6E-8C81-F21FBC4EE85D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A311D61-01C7-4112-B3DC-EA4C8351F416}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t xml:space="preserve">Expenses </t>
   </si>
@@ -142,6 +148,33 @@
   </si>
   <si>
     <t xml:space="preserve">Kickstand </t>
+  </si>
+  <si>
+    <t>https://www.mopeddivision.com/tomos-a35-center-kickstand/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kickstand Center Spring </t>
+  </si>
+  <si>
+    <t>https://www.mopeddivision.com/tomos-center-stand-spring-replacement/</t>
+  </si>
+  <si>
+    <t>Mirrors</t>
+  </si>
+  <si>
+    <t>https://www.mopeddivision.com/kinetic-moped-rectangular-threaded-10mm-mirror-set-universal-black-chrome/</t>
+  </si>
+  <si>
+    <t>tbd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tbd. </t>
+  </si>
+  <si>
+    <t>https://www.unh.edu/transportation/moped-permits</t>
+  </si>
+  <si>
+    <t>https://www.nh.gov/safety/divisions/dmv/registration/index.htm</t>
   </si>
 </sst>
 </file>
@@ -539,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B20:H48"/>
+  <dimension ref="B20:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -724,26 +757,74 @@
       <c r="C38" t="s">
         <v>23</v>
       </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
         <v>24</v>
       </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
         <v>25</v>
       </c>
+      <c r="D40" s="2">
+        <v>30</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
         <v>26</v>
       </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
         <v>27</v>
       </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
@@ -833,6 +914,52 @@
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
         <v>38</v>
+      </c>
+      <c r="D48" s="2">
+        <v>20</v>
+      </c>
+      <c r="E48" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" s="2">
+        <v>4</v>
+      </c>
+      <c r="E49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" s="2">
+        <v>37</v>
+      </c>
+      <c r="E50" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -845,8 +972,13 @@
     <hyperlink ref="G45" r:id="rId6" xr:uid="{1CB963D5-652C-45FA-A17A-F04E4944720B}"/>
     <hyperlink ref="G47" r:id="rId7" xr:uid="{0A7C3CDF-49B0-4B17-B494-B57BA5EAE805}"/>
     <hyperlink ref="G46" r:id="rId8" xr:uid="{E3B96414-2DA7-4716-85A0-573137AEBB7D}"/>
+    <hyperlink ref="G48" r:id="rId9" xr:uid="{C6BD6FEC-1AEE-4259-B430-28B4458E9116}"/>
+    <hyperlink ref="G49" r:id="rId10" xr:uid="{E853ED4D-56B7-445B-BB28-F039C4F4948F}"/>
+    <hyperlink ref="G50" r:id="rId11" xr:uid="{CAE10242-95FD-48D2-9250-97BA92EFFE8B}"/>
+    <hyperlink ref="G40" r:id="rId12" xr:uid="{3EFED318-E937-45AB-9CDE-CC224A1D4D2B}"/>
+    <hyperlink ref="G39" r:id="rId13" xr:uid="{F110C8D7-3CB4-49E9-93F7-19DBC3B362BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId9"/>
+  <drawing r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>